<commit_message>
Update qualitative analysis with codes counting.
</commit_message>
<xml_diff>
--- a/demographics.xlsx
+++ b/demographics.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F638777-9425-4758-9DD5-BAFFA23E72C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D60BC59-49BC-4F94-88C1-E0D1A6ECBB87}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="147">
   <si>
     <t>Programming Experience</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Duplo</t>
   </si>
   <si>
-    <t>RSOY</t>
-  </si>
-  <si>
     <t>1 to 2 years</t>
   </si>
   <si>
@@ -373,6 +370,102 @@
   </si>
   <si>
     <t>Mechanical Engineering, Bachelor of Science</t>
+  </si>
+  <si>
+    <t>Biology</t>
+  </si>
+  <si>
+    <t>Cinema</t>
+  </si>
+  <si>
+    <t>Music</t>
+  </si>
+  <si>
+    <t>Computer-Science</t>
+  </si>
+  <si>
+    <t>Philosophy</t>
+  </si>
+  <si>
+    <t>Communication-Arts</t>
+  </si>
+  <si>
+    <t>Physical-Therapy</t>
+  </si>
+  <si>
+    <t>Counselor-Education</t>
+  </si>
+  <si>
+    <t>Mechanical-Engineering</t>
+  </si>
+  <si>
+    <t>Mechanical-and-Nuclear-Engineering</t>
+  </si>
+  <si>
+    <t>Dentistry</t>
+  </si>
+  <si>
+    <t>Electrical-Engineering</t>
+  </si>
+  <si>
+    <t>Nursing</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>Computer-Engineering</t>
+  </si>
+  <si>
+    <t>Forensic-Science</t>
+  </si>
+  <si>
+    <t>Criminal-Justice</t>
+  </si>
+  <si>
+    <t>Accounting</t>
+  </si>
+  <si>
+    <t>Information-Systems</t>
+  </si>
+  <si>
+    <t>Sculpture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Communication-Arts </t>
+  </si>
+  <si>
+    <t>Clinical-Radiation-Sciences</t>
+  </si>
+  <si>
+    <t>Health-Sciences</t>
+  </si>
+  <si>
+    <t>Environmental-Studies</t>
+  </si>
+  <si>
+    <t>Kinetic-Imaging</t>
+  </si>
+  <si>
+    <t>Mathematical-Sciences</t>
+  </si>
+  <si>
+    <t>Bioinformatics</t>
+  </si>
+  <si>
+    <t>Physical-Education-and-Exercise-Science</t>
+  </si>
+  <si>
+    <t>Biomedical-Engineering</t>
+  </si>
+  <si>
+    <t>Physics</t>
+  </si>
+  <si>
+    <t>Political-Science</t>
+  </si>
+  <si>
+    <t>ROY</t>
   </si>
 </sst>
 </file>
@@ -466,7 +559,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -486,6 +579,15 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -495,17 +597,11 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -632,7 +728,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>RSOY</c:v>
+                  <c:v>ROY</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1747,7 +1843,7 @@
   <dimension ref="A1:P46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:K2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1775,22 +1871,22 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="9"/>
+      <c r="C2" s="12"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="10"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="11"/>
+      <c r="K2" s="14"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -1802,24 +1898,24 @@
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>4</v>
+      <c r="C3" s="16" t="s">
+        <v>146</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>4</v>
+      <c r="G3" s="16" t="s">
+        <v>146</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>4</v>
+      <c r="K3" s="16" t="s">
+        <v>146</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -1830,26 +1926,26 @@
     <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>6</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -1860,26 +1956,26 @@
     <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -1890,26 +1986,26 @@
     <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
@@ -1920,26 +2016,26 @@
     <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -1950,26 +2046,26 @@
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
@@ -1980,26 +2076,26 @@
     <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
@@ -2010,26 +2106,26 @@
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
@@ -2040,26 +2136,26 @@
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
@@ -2070,26 +2166,26 @@
     <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
@@ -2100,26 +2196,26 @@
     <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
@@ -2130,26 +2226,26 @@
     <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
@@ -2160,26 +2256,26 @@
     <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
@@ -2190,26 +2286,26 @@
     <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
@@ -2220,26 +2316,26 @@
     <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
@@ -2250,26 +2346,26 @@
     <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
@@ -2280,26 +2376,26 @@
     <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
@@ -2310,26 +2406,26 @@
     <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
@@ -2340,26 +2436,26 @@
     <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
@@ -2370,26 +2466,26 @@
     <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
@@ -2400,26 +2496,26 @@
     <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
@@ -2430,26 +2526,26 @@
     <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
@@ -2460,26 +2556,26 @@
     <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
@@ -2490,26 +2586,26 @@
     <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
@@ -2520,26 +2616,26 @@
     <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
       <c r="B27" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
@@ -2550,26 +2646,26 @@
     <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
       <c r="B28" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
@@ -2580,26 +2676,26 @@
     <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="B29" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
@@ -2627,22 +2723,22 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
-      <c r="B31" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C31" s="9"/>
+      <c r="B31" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="12"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
-      <c r="F31" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G31" s="10"/>
+      <c r="F31" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G31" s="13"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
-      <c r="J31" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="K31" s="11"/>
+      <c r="J31" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="K31" s="14"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
@@ -2654,24 +2750,24 @@
       <c r="B32" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>4</v>
+      <c r="C32" s="16" t="s">
+        <v>146</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G32" s="2" t="s">
-        <v>4</v>
+      <c r="G32" s="16" t="s">
+        <v>146</v>
       </c>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K32" s="2" t="s">
-        <v>4</v>
+      <c r="K32" s="16" t="s">
+        <v>146</v>
       </c>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
@@ -2681,7 +2777,7 @@
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B33" s="1">
         <f>COUNTIF(B4:B29, A33)</f>
@@ -2693,7 +2789,7 @@
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F33" s="6">
         <f>COUNTIF(F4:F29, E33) / 26</f>
@@ -2705,7 +2801,7 @@
       </c>
       <c r="H33" s="1"/>
       <c r="I33" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J33" s="7">
         <f>COUNTIF(J4:J29, I33) / 26</f>
@@ -2723,7 +2819,7 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B34" s="1">
         <f>COUNTIF(B4:B29, A34)</f>
@@ -2735,7 +2831,7 @@
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F34" s="6">
         <f>COUNTIF(F4:F29, E34) / 26</f>
@@ -2747,7 +2843,7 @@
       </c>
       <c r="H34" s="1"/>
       <c r="I34" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J34" s="7">
         <f>COUNTIF(J4:J29, I34) / 26</f>
@@ -2765,7 +2861,7 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B35" s="1">
         <f>COUNTIF(B4:B29, A35)</f>
@@ -2791,7 +2887,7 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B36" s="1">
         <f>COUNTIF(B4:B29, A36)</f>
@@ -2817,7 +2913,7 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B37" s="1">
         <f>COUNTIF(B4:B29, A37)</f>
@@ -3019,10 +3115,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54D3EFC3-74D3-4422-87F3-835F160D49F7}">
-  <dimension ref="A1:I87"/>
+  <dimension ref="A1:I146"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C95" sqref="C95:C146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3034,70 +3130,70 @@
   <sheetData>
     <row r="1" spans="1:9" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>16</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>17</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="G1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="8" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="4">
         <v>18</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I3" s="4">
         <v>5.1388888888888887E-2</v>
@@ -3105,28 +3201,28 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="4">
         <v>20</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I4" s="4">
         <v>6.3888888888888884E-2</v>
@@ -3134,28 +3230,28 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" s="4">
         <v>18</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>3</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I5" s="4">
         <v>7.2916666666666671E-2</v>
@@ -3163,28 +3259,28 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="4">
         <v>18</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>33</v>
-      </c>
       <c r="E6" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I6" s="4">
         <v>3.6805555555555557E-2</v>
@@ -3192,28 +3288,28 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" s="4">
         <v>19</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>36</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>3</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I7" s="4">
         <v>3.3333333333333333E-2</v>
@@ -3221,28 +3317,28 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" s="4">
         <v>19</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>3</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I8" s="4">
         <v>7.2916666666666671E-2</v>
@@ -3250,28 +3346,28 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" s="4">
         <v>20</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>3</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I9" s="4">
         <v>2.361111111111111E-2</v>
@@ -3279,28 +3375,28 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" s="4">
         <v>19</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>3</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I10" s="4">
         <v>4.2361111111111113E-2</v>
@@ -3308,28 +3404,28 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11" s="4">
         <v>20</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>3</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I11" s="4">
         <v>7.2916666666666671E-2</v>
@@ -3337,28 +3433,28 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B12" s="4">
         <v>23</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>3</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I12" s="4">
         <v>4.8611111111111112E-2</v>
@@ -3366,28 +3462,28 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B13" s="4">
         <v>32</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>3</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I13" s="4">
         <v>7.2916666666666671E-2</v>
@@ -3395,28 +3491,28 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="4">
+        <v>22</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="4">
-        <v>22</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>46</v>
-      </c>
       <c r="D14" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>3</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I14" s="4">
         <v>5.9027777777777776E-2</v>
@@ -3424,28 +3520,28 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="4">
+        <v>22</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="4">
-        <v>22</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>48</v>
-      </c>
       <c r="D15" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>3</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I15" s="4">
         <v>2.9166666666666667E-2</v>
@@ -3453,28 +3549,28 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B16" s="4">
         <v>18</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>3</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I16" s="4">
         <v>3.8194444444444448E-2</v>
@@ -3482,28 +3578,28 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B17" s="4">
         <v>25</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>3</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I17" s="4">
         <v>4.583333333333333E-2</v>
@@ -3511,28 +3607,28 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B18" s="4">
         <v>20</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>3</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I18" s="4">
         <v>2.1527777777777778E-2</v>
@@ -3540,28 +3636,28 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B19" s="4">
         <v>24</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>3</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I19" s="4">
         <v>3.3333333333333333E-2</v>
@@ -3569,28 +3665,28 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B20" s="4">
         <v>19</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>3</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I20" s="4">
         <v>1.9444444444444445E-2</v>
@@ -3598,28 +3694,28 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B21" s="4">
         <v>31</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>3</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I21" s="4">
         <v>6.5277777777777782E-2</v>
@@ -3627,28 +3723,28 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B22" s="4">
         <v>23</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>3</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I22" s="4">
         <v>7.2916666666666671E-2</v>
@@ -3656,28 +3752,28 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B23" s="4">
         <v>21</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>3</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I23" s="4">
         <v>2.9861111111111113E-2</v>
@@ -3685,28 +3781,28 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B24" s="4">
         <v>19</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>3</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I24" s="4">
         <v>5.4166666666666669E-2</v>
@@ -3714,28 +3810,28 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B25" s="4">
         <v>23</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D25" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>3</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I25" s="4">
         <v>6.7361111111111108E-2</v>
@@ -3743,28 +3839,28 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B26" s="4">
         <v>24</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>3</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I26" s="4">
         <v>3.4027777777777775E-2</v>
@@ -3772,28 +3868,28 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B27" s="4">
         <v>19</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>3</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I27" s="4">
         <v>2.2222222222222223E-2</v>
@@ -3801,70 +3897,70 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B28" s="4">
         <v>23</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E28" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F28" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>3</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I28" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="14"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
+      <c r="A29" s="10"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B30" s="4">
         <v>27</v>
       </c>
       <c r="C30" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G30" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>73</v>
-      </c>
       <c r="H30" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I30" s="4">
         <v>7.2916666666666671E-2</v>
@@ -3872,28 +3968,28 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B31" s="4">
         <v>20</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I31" s="4">
         <v>5.6250000000000001E-2</v>
@@ -3901,28 +3997,28 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B32" s="4">
+        <v>22</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B32" s="4">
-        <v>22</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>77</v>
-      </c>
       <c r="D32" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I32" s="4">
         <v>7.2916666666666671E-2</v>
@@ -3930,28 +4026,28 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B33" s="4">
         <v>21</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I33" s="4">
         <v>7.2916666666666671E-2</v>
@@ -3959,28 +4055,28 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B34" s="4">
         <v>28</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D34" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F34" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E34" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="G34" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I34" s="4">
         <v>7.2916666666666671E-2</v>
@@ -3988,28 +4084,28 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B35" s="4">
         <v>18</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I35" s="4">
         <v>2.4305555555555556E-2</v>
@@ -4017,28 +4113,28 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B36" s="4">
         <v>18</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I36" s="4">
         <v>6.0416666666666667E-2</v>
@@ -4046,28 +4142,28 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B37" s="4">
         <v>21</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I37" s="4">
         <v>6.1805555555555558E-2</v>
@@ -4075,28 +4171,28 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B38" s="4">
         <v>22</v>
       </c>
       <c r="C38" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="H38" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G38" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="H38" s="4" t="s">
-        <v>30</v>
       </c>
       <c r="I38" s="4">
         <v>7.2916666666666671E-2</v>
@@ -4104,28 +4200,28 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B39" s="4">
         <v>48</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I39" s="4">
         <v>7.2916666666666671E-2</v>
@@ -4133,28 +4229,28 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B40" s="4">
         <v>19</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I40" s="4">
         <v>7.2916666666666671E-2</v>
@@ -4162,28 +4258,28 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B41" s="4">
         <v>18</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I41" s="4">
         <v>7.2916666666666671E-2</v>
@@ -4191,28 +4287,28 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B42" s="4">
         <v>19</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I42" s="4">
         <v>7.2916666666666671E-2</v>
@@ -4220,28 +4316,28 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B43" s="4">
         <v>34</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I43" s="4">
         <v>5.1388888888888887E-2</v>
@@ -4249,28 +4345,28 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B44" s="4">
         <v>26</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I44" s="4">
         <v>7.2916666666666671E-2</v>
@@ -4278,28 +4374,28 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B45" s="4">
         <v>50</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I45" s="4">
         <v>7.2916666666666671E-2</v>
@@ -4307,28 +4403,28 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B46" s="4">
         <v>22</v>
       </c>
       <c r="C46" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G46" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D46" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F46" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G46" s="4" t="s">
-        <v>73</v>
-      </c>
       <c r="H46" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I46" s="4">
         <v>6.3888888888888884E-2</v>
@@ -4336,28 +4432,28 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B47" s="4">
         <v>19</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I47" s="4">
         <v>4.8611111111111112E-2</v>
@@ -4365,28 +4461,28 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B48" s="4">
         <v>18</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I48" s="4">
         <v>5.2083333333333336E-2</v>
@@ -4394,28 +4490,28 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B49" s="4">
         <v>20</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I49" s="4">
         <v>3.9583333333333331E-2</v>
@@ -4423,28 +4519,28 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B50" s="4">
+        <v>22</v>
+      </c>
+      <c r="C50" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B50" s="4">
-        <v>22</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>104</v>
-      </c>
       <c r="D50" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F50" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E50" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F50" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="G50" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I50" s="4">
         <v>7.2916666666666671E-2</v>
@@ -4452,28 +4548,28 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B51" s="4">
         <v>32</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I51" s="4">
         <v>7.2916666666666671E-2</v>
@@ -4481,28 +4577,28 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B52" s="4">
         <v>17</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I52" s="4">
         <v>7.2916666666666671E-2</v>
@@ -4510,28 +4606,28 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B53" s="4">
         <v>20</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I53" s="4">
         <v>6.1805555555555558E-2</v>
@@ -4539,28 +4635,28 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B54" s="4">
         <v>21</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D54" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F54" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E54" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F54" s="4" t="s">
+      <c r="G54" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="H54" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="G54" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="H54" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="I54" s="4">
         <v>5.9722222222222225E-2</v>
@@ -4568,186 +4664,446 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B55" s="4">
         <v>19</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H55" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I55" s="4">
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C57" s="12" t="s">
-        <v>113</v>
+      <c r="C57" s="9" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C58" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C59" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C60" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C61" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C62" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C63" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C64" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="65" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C65" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="66" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C66" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="67" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C67" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="68" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C68" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="69" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C69" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="70" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C70" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="71" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C71" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="72" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C72" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="73" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C73" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="74" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C74" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="75" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C75" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="76" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C76" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="77" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C77" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="78" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C78" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="79" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C79" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="80" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C80" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="81" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C81" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="82" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C82" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="83" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C83" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="84" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C84" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="85" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C85" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="86" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C86" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="87" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C87" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="95" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C95" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="96" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C96" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="97" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C97" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="98" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C98" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="99" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C99" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="100" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C100" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="101" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C101" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="102" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C102" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="103" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C103" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="104" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C104" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="105" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C105" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="106" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C106" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="107" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C107" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="108" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C108" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="109" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C109" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="110" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C110" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="111" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C111" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="112" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C112" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="113" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C113" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="114" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C114" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="115" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C115" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="116" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C116" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="117" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C117" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="118" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C118" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="119" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C119" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="120" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C120" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="121" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C121" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="122" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C122" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="123" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C123" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="124" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C124" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="125" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C125" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="126" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C126" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="127" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C127" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="128" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C128" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="129" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C129" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="130" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C130" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="131" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C131" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="132" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C132" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="133" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C133" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="134" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C134" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="135" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C135" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="136" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C136" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="137" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C137" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="138" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C138" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="139" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C139" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="140" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C140" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="141" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C141" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="142" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C142" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="143" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C143" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="144" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C144" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="145" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C145" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="146" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C146" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More updates on data analysis.
</commit_message>
<xml_diff>
--- a/demographics.xlsx
+++ b/demographics.xlsx
@@ -3,17 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D60BC59-49BC-4F94-88C1-E0D1A6ECBB87}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA4E1F5B-7AD0-495E-B503-DA372E0BF7D8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7913" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demographics" sheetId="1" r:id="rId1"/>
     <sheet name="Survey Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Survey Data'!$C$3:$C$55</definedName>
-    <definedName name="_xlnm.Extract" localSheetId="1">'Survey Data'!$C$58</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Survey Data'!$C$95:$C$146</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="1">'Survey Data'!$E$95</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="147">
   <si>
     <t>Programming Experience</t>
   </si>
@@ -472,7 +472,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -494,6 +494,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="5"/>
+      <color rgb="FF454545"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="9">
@@ -559,7 +565,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -588,6 +594,9 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -600,9 +609,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1842,16 +1849,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="11" width="20.6328125" customWidth="1"/>
+    <col min="1" max="11" width="20.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1869,36 +1876,36 @@
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A2" s="1"/>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12"/>
+      <c r="C2" s="13"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="13"/>
+      <c r="G2" s="14"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
-      <c r="J2" s="14" t="s">
+      <c r="J2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="14"/>
+      <c r="K2" s="15"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="12" t="s">
         <v>146</v>
       </c>
       <c r="D3" s="1"/>
@@ -1906,7 +1913,7 @@
       <c r="F3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="12" t="s">
         <v>146</v>
       </c>
       <c r="H3" s="1"/>
@@ -1914,7 +1921,7 @@
       <c r="J3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="16" t="s">
+      <c r="K3" s="12" t="s">
         <v>146</v>
       </c>
       <c r="L3" s="1"/>
@@ -1923,7 +1930,7 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A4" s="1"/>
       <c r="B4" s="3" t="s">
         <v>4</v>
@@ -1953,7 +1960,7 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A5" s="1"/>
       <c r="B5" s="3" t="s">
         <v>7</v>
@@ -1983,7 +1990,7 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
         <v>7</v>
@@ -2013,7 +2020,7 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A7" s="1"/>
       <c r="B7" s="3" t="s">
         <v>8</v>
@@ -2043,7 +2050,7 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A8" s="1"/>
       <c r="B8" s="3" t="s">
         <v>5</v>
@@ -2073,7 +2080,7 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A9" s="1"/>
       <c r="B9" s="3" t="s">
         <v>7</v>
@@ -2103,7 +2110,7 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A10" s="1"/>
       <c r="B10" s="5" t="s">
         <v>10</v>
@@ -2133,7 +2140,7 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A11" s="1"/>
       <c r="B11" s="3" t="s">
         <v>7</v>
@@ -2163,7 +2170,7 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A12" s="1"/>
       <c r="B12" s="3" t="s">
         <v>7</v>
@@ -2193,7 +2200,7 @@
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A13" s="1"/>
       <c r="B13" s="3" t="s">
         <v>7</v>
@@ -2223,7 +2230,7 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A14" s="1"/>
       <c r="B14" s="3" t="s">
         <v>4</v>
@@ -2253,7 +2260,7 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A15" s="1"/>
       <c r="B15" s="3" t="s">
         <v>8</v>
@@ -2283,7 +2290,7 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A16" s="1"/>
       <c r="B16" s="3" t="s">
         <v>5</v>
@@ -2313,7 +2320,7 @@
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A17" s="1"/>
       <c r="B17" s="3" t="s">
         <v>8</v>
@@ -2343,7 +2350,7 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A18" s="1"/>
       <c r="B18" s="3" t="s">
         <v>7</v>
@@ -2373,7 +2380,7 @@
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A19" s="1"/>
       <c r="B19" s="3" t="s">
         <v>8</v>
@@ -2403,7 +2410,7 @@
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A20" s="1"/>
       <c r="B20" s="3" t="s">
         <v>7</v>
@@ -2433,7 +2440,7 @@
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A21" s="1"/>
       <c r="B21" s="3" t="s">
         <v>8</v>
@@ -2463,7 +2470,7 @@
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A22" s="1"/>
       <c r="B22" s="3" t="s">
         <v>8</v>
@@ -2493,7 +2500,7 @@
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A23" s="1"/>
       <c r="B23" s="3" t="s">
         <v>7</v>
@@ -2523,7 +2530,7 @@
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A24" s="1"/>
       <c r="B24" s="3" t="s">
         <v>5</v>
@@ -2553,7 +2560,7 @@
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A25" s="1"/>
       <c r="B25" s="3" t="s">
         <v>8</v>
@@ -2583,7 +2590,7 @@
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A26" s="1"/>
       <c r="B26" s="3" t="s">
         <v>4</v>
@@ -2613,7 +2620,7 @@
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A27" s="1"/>
       <c r="B27" s="3" t="s">
         <v>5</v>
@@ -2643,7 +2650,7 @@
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A28" s="1"/>
       <c r="B28" s="3" t="s">
         <v>7</v>
@@ -2673,7 +2680,7 @@
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A29" s="1"/>
       <c r="B29" s="3" t="s">
         <v>4</v>
@@ -2703,7 +2710,7 @@
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -2721,36 +2728,36 @@
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A31" s="1"/>
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C31" s="12"/>
+      <c r="C31" s="13"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
-      <c r="F31" s="13" t="s">
+      <c r="F31" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G31" s="13"/>
+      <c r="G31" s="14"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
-      <c r="J31" s="14" t="s">
+      <c r="J31" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="K31" s="14"/>
+      <c r="K31" s="15"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A32" s="1"/>
       <c r="B32" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C32" s="16" t="s">
+      <c r="C32" s="12" t="s">
         <v>146</v>
       </c>
       <c r="D32" s="1"/>
@@ -2758,7 +2765,7 @@
       <c r="F32" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G32" s="16" t="s">
+      <c r="G32" s="12" t="s">
         <v>146</v>
       </c>
       <c r="H32" s="1"/>
@@ -2766,7 +2773,7 @@
       <c r="J32" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K32" s="16" t="s">
+      <c r="K32" s="12" t="s">
         <v>146</v>
       </c>
       <c r="L32" s="1"/>
@@ -2775,7 +2782,7 @@
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A33" s="3" t="s">
         <v>7</v>
       </c>
@@ -2817,7 +2824,7 @@
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A34" s="3" t="s">
         <v>8</v>
       </c>
@@ -2859,7 +2866,7 @@
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A35" s="3" t="s">
         <v>4</v>
       </c>
@@ -2885,7 +2892,7 @@
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A36" s="3" t="s">
         <v>5</v>
       </c>
@@ -2911,7 +2918,7 @@
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A37" s="5" t="s">
         <v>10</v>
       </c>
@@ -2937,7 +2944,7 @@
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -2955,7 +2962,7 @@
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -2973,7 +2980,7 @@
       <c r="O39" s="1"/>
       <c r="P39" s="1"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -2991,7 +2998,7 @@
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -3009,7 +3016,7 @@
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -3027,7 +3034,7 @@
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -3045,7 +3052,7 @@
       <c r="O43" s="1"/>
       <c r="P43" s="1"/>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -3063,7 +3070,7 @@
       <c r="O44" s="1"/>
       <c r="P44" s="1"/>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -3081,7 +3088,7 @@
       <c r="O45" s="1"/>
       <c r="P45" s="1"/>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -3115,20 +3122,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54D3EFC3-74D3-4422-87F3-835F160D49F7}">
-  <dimension ref="A1:I146"/>
+  <dimension ref="A1:I147"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C95" sqref="C95:C146"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="F105" sqref="F105:F106"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="5" width="20.6328125" customWidth="1"/>
-    <col min="6" max="6" width="24.1796875" customWidth="1"/>
-    <col min="7" max="9" width="20.6328125" customWidth="1"/>
+    <col min="1" max="5" width="20.59765625" customWidth="1"/>
+    <col min="6" max="6" width="24.19921875" customWidth="1"/>
+    <col min="7" max="9" width="20.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="8" t="s">
         <v>12</v>
       </c>
@@ -3157,20 +3164,20 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>20</v>
       </c>
@@ -3199,7 +3206,7 @@
         <v>5.1388888888888887E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>25</v>
       </c>
@@ -3228,7 +3235,7 @@
         <v>6.3888888888888884E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>27</v>
       </c>
@@ -3257,7 +3264,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>30</v>
       </c>
@@ -3286,7 +3293,7 @@
         <v>3.6805555555555557E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>33</v>
       </c>
@@ -3315,7 +3322,7 @@
         <v>3.3333333333333333E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
         <v>36</v>
       </c>
@@ -3344,7 +3351,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="4" t="s">
         <v>37</v>
       </c>
@@ -3373,7 +3380,7 @@
         <v>2.361111111111111E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="s">
         <v>39</v>
       </c>
@@ -3402,7 +3409,7 @@
         <v>4.2361111111111113E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="4" t="s">
         <v>40</v>
       </c>
@@ -3431,7 +3438,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="4" t="s">
         <v>42</v>
       </c>
@@ -3460,7 +3467,7 @@
         <v>4.8611111111111112E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="4" t="s">
         <v>43</v>
       </c>
@@ -3489,7 +3496,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="4" t="s">
         <v>44</v>
       </c>
@@ -3518,7 +3525,7 @@
         <v>5.9027777777777776E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="4" t="s">
         <v>46</v>
       </c>
@@ -3547,7 +3554,7 @@
         <v>2.9166666666666667E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
         <v>48</v>
       </c>
@@ -3576,7 +3583,7 @@
         <v>3.8194444444444448E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="4" t="s">
         <v>49</v>
       </c>
@@ -3605,7 +3612,7 @@
         <v>4.583333333333333E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="4" t="s">
         <v>51</v>
       </c>
@@ -3634,7 +3641,7 @@
         <v>2.1527777777777778E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="4" t="s">
         <v>53</v>
       </c>
@@ -3663,7 +3670,7 @@
         <v>3.3333333333333333E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="4" t="s">
         <v>54</v>
       </c>
@@ -3692,7 +3699,7 @@
         <v>1.9444444444444445E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" s="4" t="s">
         <v>56</v>
       </c>
@@ -3721,7 +3728,7 @@
         <v>6.5277777777777782E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" s="4" t="s">
         <v>58</v>
       </c>
@@ -3750,7 +3757,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="4" t="s">
         <v>59</v>
       </c>
@@ -3779,7 +3786,7 @@
         <v>2.9861111111111113E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="4" t="s">
         <v>61</v>
       </c>
@@ -3808,7 +3815,7 @@
         <v>5.4166666666666669E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" s="4" t="s">
         <v>63</v>
       </c>
@@ -3837,7 +3844,7 @@
         <v>6.7361111111111108E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" s="4" t="s">
         <v>65</v>
       </c>
@@ -3866,7 +3873,7 @@
         <v>3.4027777777777775E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" s="4" t="s">
         <v>66</v>
       </c>
@@ -3895,7 +3902,7 @@
         <v>2.2222222222222223E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" s="4" t="s">
         <v>68</v>
       </c>
@@ -3924,7 +3931,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="10"/>
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
@@ -3937,7 +3944,7 @@
       <c r="H29" s="10"/>
       <c r="I29" s="10"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" s="4" t="s">
         <v>70</v>
       </c>
@@ -3966,7 +3973,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" s="4" t="s">
         <v>73</v>
       </c>
@@ -3995,7 +4002,7 @@
         <v>5.6250000000000001E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32" s="4" t="s">
         <v>75</v>
       </c>
@@ -4024,7 +4031,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" s="4" t="s">
         <v>77</v>
       </c>
@@ -4053,7 +4060,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A34" s="4" t="s">
         <v>79</v>
       </c>
@@ -4082,7 +4089,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" s="4" t="s">
         <v>81</v>
       </c>
@@ -4111,7 +4118,7 @@
         <v>2.4305555555555556E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" s="4" t="s">
         <v>82</v>
       </c>
@@ -4140,7 +4147,7 @@
         <v>6.0416666666666667E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37" s="4" t="s">
         <v>84</v>
       </c>
@@ -4169,7 +4176,7 @@
         <v>6.1805555555555558E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38" s="4" t="s">
         <v>85</v>
       </c>
@@ -4198,7 +4205,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A39" s="4" t="s">
         <v>86</v>
       </c>
@@ -4227,7 +4234,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A40" s="4" t="s">
         <v>88</v>
       </c>
@@ -4256,7 +4263,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A41" s="4" t="s">
         <v>89</v>
       </c>
@@ -4285,7 +4292,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A42" s="4" t="s">
         <v>91</v>
       </c>
@@ -4314,7 +4321,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A43" s="4" t="s">
         <v>93</v>
       </c>
@@ -4343,7 +4350,7 @@
         <v>5.1388888888888887E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A44" s="4" t="s">
         <v>94</v>
       </c>
@@ -4372,7 +4379,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A45" s="4" t="s">
         <v>95</v>
       </c>
@@ -4401,7 +4408,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A46" s="4" t="s">
         <v>96</v>
       </c>
@@ -4430,7 +4437,7 @@
         <v>6.3888888888888884E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A47" s="4" t="s">
         <v>97</v>
       </c>
@@ -4459,7 +4466,7 @@
         <v>4.8611111111111112E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A48" s="4" t="s">
         <v>99</v>
       </c>
@@ -4488,7 +4495,7 @@
         <v>5.2083333333333336E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49" s="4" t="s">
         <v>100</v>
       </c>
@@ -4517,7 +4524,7 @@
         <v>3.9583333333333331E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50" s="4" t="s">
         <v>102</v>
       </c>
@@ -4546,7 +4553,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A51" s="4" t="s">
         <v>104</v>
       </c>
@@ -4575,7 +4582,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A52" s="4" t="s">
         <v>105</v>
       </c>
@@ -4604,7 +4611,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A53" s="4" t="s">
         <v>107</v>
       </c>
@@ -4633,7 +4640,7 @@
         <v>6.1805555555555558E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A54" s="4" t="s">
         <v>108</v>
       </c>
@@ -4662,7 +4669,7 @@
         <v>5.9722222222222225E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A55" s="4" t="s">
         <v>110</v>
       </c>
@@ -4691,425 +4698,646 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C57" s="9" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C58" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C59" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C60" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C61" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C62" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C63" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C64" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C65" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C66" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C67" s="4" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C68" s="4" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C69" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C70" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C71" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C72" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C73" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="74" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C74" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C75" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="76" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C76" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C77" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="78" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C78" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="79" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C79" s="4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="80" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="80" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C80" s="4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C81" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="82" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C82" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="83" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="83" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C83" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="84" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="84" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C84" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="85" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="85" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C85" s="4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="86" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="86" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C86" s="4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="87" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="87" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C87" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="95" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="95" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C95" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="96" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="E95" t="s">
+        <v>118</v>
+      </c>
+      <c r="F95">
+        <f>COUNTIF(C$95:C$146,E95)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C96" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="E96" t="s">
+        <v>145</v>
+      </c>
+      <c r="F96">
+        <f t="shared" ref="F96:F126" si="0">COUNTIF(C$95:C$146,E96)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C97" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="98" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="E97" t="s">
+        <v>115</v>
+      </c>
+      <c r="F97">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="98" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C98" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="99" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="E98" t="s">
+        <v>116</v>
+      </c>
+      <c r="F98">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="99" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C99" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="100" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="E99" t="s">
+        <v>117</v>
+      </c>
+      <c r="F99">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C100" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="101" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="101" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C101" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="102" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="E101" t="s">
+        <v>119</v>
+      </c>
+      <c r="F101">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C102" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="103" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="E102" t="s">
+        <v>120</v>
+      </c>
+      <c r="F102">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C103" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="104" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="E103" t="s">
+        <v>121</v>
+      </c>
+      <c r="F103">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C104" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="105" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="E104" t="s">
+        <v>122</v>
+      </c>
+      <c r="F104">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C105" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="106" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="E105" t="s">
+        <v>123</v>
+      </c>
+      <c r="F105">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="106" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C106" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="107" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="E106" t="s">
+        <v>124</v>
+      </c>
+      <c r="F106">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C107" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="108" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="E107" t="s">
+        <v>125</v>
+      </c>
+      <c r="F107">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C108" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="109" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="E108" t="s">
+        <v>126</v>
+      </c>
+      <c r="F108">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="109" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C109" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="110" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="E109" t="s">
+        <v>127</v>
+      </c>
+      <c r="F109">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C110" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="111" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="E110" t="s">
+        <v>128</v>
+      </c>
+      <c r="F110">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C111" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="112" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="E111" t="s">
+        <v>129</v>
+      </c>
+      <c r="F111">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C112" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="113" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="E112" t="s">
+        <v>130</v>
+      </c>
+      <c r="F112">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C113" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="114" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="E113" t="s">
+        <v>131</v>
+      </c>
+      <c r="F113">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C114" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="115" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="E114" t="s">
+        <v>132</v>
+      </c>
+      <c r="F114">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="115" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C115" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="116" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="E115" t="s">
+        <v>133</v>
+      </c>
+      <c r="F115">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C116" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="117" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="E116" t="s">
+        <v>134</v>
+      </c>
+      <c r="F116">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C117" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="118" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="E117" t="s">
+        <v>135</v>
+      </c>
+      <c r="F117">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C118" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="119" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="E118" t="s">
+        <v>136</v>
+      </c>
+      <c r="F118">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C119" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="120" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="E119" t="s">
+        <v>137</v>
+      </c>
+      <c r="F119">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C120" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="121" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="E120" t="s">
+        <v>138</v>
+      </c>
+      <c r="F120">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C121" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="122" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="E121" t="s">
+        <v>139</v>
+      </c>
+      <c r="F121">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C122" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="123" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="E122" t="s">
+        <v>140</v>
+      </c>
+      <c r="F122">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C123" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="124" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="E123" t="s">
+        <v>141</v>
+      </c>
+      <c r="F123">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C124" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="125" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="E124" t="s">
+        <v>142</v>
+      </c>
+      <c r="F124">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C125" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="126" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="E125" t="s">
+        <v>143</v>
+      </c>
+      <c r="F125">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C126" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="127" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="E126" t="s">
+        <v>144</v>
+      </c>
+      <c r="F126">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C127" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="128" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="128" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C128" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="129" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="129" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C129" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="130" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="130" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C130" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="131" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="131" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C131" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="132" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="132" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C132" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="133" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="133" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C133" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="134" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="134" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C134" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="135" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="135" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C135" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="136" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="136" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C136" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="137" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="137" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C137" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="138" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="138" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C138" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="139" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="139" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C139" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="140" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="140" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C140" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="141" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="141" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C141" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="142" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="142" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C142" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="143" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="143" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C143" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="144" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="144" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C144" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="145" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="145" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C145" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="146" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="146" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C146" t="s">
         <v>144</v>
       </c>
+    </row>
+    <row r="147" spans="3:3" x14ac:dyDescent="0.45">
+      <c r="C147" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updates on data analysis.
</commit_message>
<xml_diff>
--- a/demographics.xlsx
+++ b/demographics.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA4E1F5B-7AD0-495E-B503-DA372E0BF7D8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F321996-C740-48A9-93AC-6C3DF7FBE6FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7913" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7910" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demographics" sheetId="1" r:id="rId1"/>
@@ -597,6 +597,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -609,7 +610,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1853,12 +1853,12 @@
       <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="11" width="20.59765625" customWidth="1"/>
+    <col min="1" max="11" width="20.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1876,31 +1876,31 @@
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13"/>
+      <c r="C2" s="14"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="15"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
-      <c r="J2" s="15" t="s">
+      <c r="J2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="15"/>
+      <c r="K2" s="16"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
         <v>3</v>
@@ -1930,7 +1930,7 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="3" t="s">
         <v>4</v>
@@ -1960,7 +1960,7 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="3" t="s">
         <v>7</v>
@@ -1990,7 +1990,7 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
         <v>7</v>
@@ -2020,7 +2020,7 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="3" t="s">
         <v>8</v>
@@ -2050,7 +2050,7 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="3" t="s">
         <v>5</v>
@@ -2080,7 +2080,7 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="3" t="s">
         <v>7</v>
@@ -2110,7 +2110,7 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="5" t="s">
         <v>10</v>
@@ -2140,7 +2140,7 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="3" t="s">
         <v>7</v>
@@ -2170,7 +2170,7 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="3" t="s">
         <v>7</v>
@@ -2200,7 +2200,7 @@
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="3" t="s">
         <v>7</v>
@@ -2230,7 +2230,7 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="3" t="s">
         <v>4</v>
@@ -2260,7 +2260,7 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="3" t="s">
         <v>8</v>
@@ -2290,7 +2290,7 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="3" t="s">
         <v>5</v>
@@ -2320,7 +2320,7 @@
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="3" t="s">
         <v>8</v>
@@ -2350,7 +2350,7 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="3" t="s">
         <v>7</v>
@@ -2380,7 +2380,7 @@
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="3" t="s">
         <v>8</v>
@@ -2410,7 +2410,7 @@
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="3" t="s">
         <v>7</v>
@@ -2440,7 +2440,7 @@
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="3" t="s">
         <v>8</v>
@@ -2470,7 +2470,7 @@
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="3" t="s">
         <v>8</v>
@@ -2500,7 +2500,7 @@
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="3" t="s">
         <v>7</v>
@@ -2530,7 +2530,7 @@
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="3" t="s">
         <v>5</v>
@@ -2560,7 +2560,7 @@
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="3" t="s">
         <v>8</v>
@@ -2590,7 +2590,7 @@
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="3" t="s">
         <v>4</v>
@@ -2620,7 +2620,7 @@
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
       <c r="B27" s="3" t="s">
         <v>5</v>
@@ -2650,7 +2650,7 @@
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
       <c r="B28" s="3" t="s">
         <v>7</v>
@@ -2680,7 +2680,7 @@
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="B29" s="3" t="s">
         <v>4</v>
@@ -2710,7 +2710,7 @@
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -2728,31 +2728,31 @@
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C31" s="13"/>
+      <c r="C31" s="14"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
-      <c r="F31" s="14" t="s">
+      <c r="F31" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="G31" s="14"/>
+      <c r="G31" s="15"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
-      <c r="J31" s="15" t="s">
+      <c r="J31" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="K31" s="15"/>
+      <c r="K31" s="16"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
       <c r="B32" s="2" t="s">
         <v>3</v>
@@ -2782,7 +2782,7 @@
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>7</v>
       </c>
@@ -2824,7 +2824,7 @@
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>8</v>
       </c>
@@ -2866,7 +2866,7 @@
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>4</v>
       </c>
@@ -2892,7 +2892,7 @@
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>5</v>
       </c>
@@ -2918,7 +2918,7 @@
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
         <v>10</v>
       </c>
@@ -2944,7 +2944,7 @@
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -2962,7 +2962,7 @@
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -2980,7 +2980,7 @@
       <c r="O39" s="1"/>
       <c r="P39" s="1"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -2998,7 +2998,7 @@
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -3016,7 +3016,7 @@
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -3034,7 +3034,7 @@
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -3052,7 +3052,7 @@
       <c r="O43" s="1"/>
       <c r="P43" s="1"/>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -3070,7 +3070,7 @@
       <c r="O44" s="1"/>
       <c r="P44" s="1"/>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -3088,7 +3088,7 @@
       <c r="O45" s="1"/>
       <c r="P45" s="1"/>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -3124,18 +3124,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54D3EFC3-74D3-4422-87F3-835F160D49F7}">
   <dimension ref="A1:I147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="F105" sqref="F105:F106"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="F130" sqref="F130"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="5" width="20.59765625" customWidth="1"/>
-    <col min="6" max="6" width="24.19921875" customWidth="1"/>
-    <col min="7" max="9" width="20.59765625" customWidth="1"/>
+    <col min="1" max="5" width="20.6328125" customWidth="1"/>
+    <col min="6" max="6" width="24.1796875" customWidth="1"/>
+    <col min="7" max="9" width="20.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>12</v>
       </c>
@@ -3164,20 +3164,20 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A2" s="16" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>20</v>
       </c>
@@ -3206,7 +3206,7 @@
         <v>5.1388888888888887E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>25</v>
       </c>
@@ -3235,7 +3235,7 @@
         <v>6.3888888888888884E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>27</v>
       </c>
@@ -3264,7 +3264,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>30</v>
       </c>
@@ -3293,7 +3293,7 @@
         <v>3.6805555555555557E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>33</v>
       </c>
@@ -3322,7 +3322,7 @@
         <v>3.3333333333333333E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>36</v>
       </c>
@@ -3351,7 +3351,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>37</v>
       </c>
@@ -3380,7 +3380,7 @@
         <v>2.361111111111111E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>39</v>
       </c>
@@ -3409,7 +3409,7 @@
         <v>4.2361111111111113E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>40</v>
       </c>
@@ -3438,7 +3438,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>42</v>
       </c>
@@ -3467,7 +3467,7 @@
         <v>4.8611111111111112E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>43</v>
       </c>
@@ -3496,7 +3496,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>44</v>
       </c>
@@ -3525,7 +3525,7 @@
         <v>5.9027777777777776E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>46</v>
       </c>
@@ -3554,7 +3554,7 @@
         <v>2.9166666666666667E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>48</v>
       </c>
@@ -3583,7 +3583,7 @@
         <v>3.8194444444444448E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>49</v>
       </c>
@@ -3612,7 +3612,7 @@
         <v>4.583333333333333E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>51</v>
       </c>
@@ -3641,7 +3641,7 @@
         <v>2.1527777777777778E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>53</v>
       </c>
@@ -3670,7 +3670,7 @@
         <v>3.3333333333333333E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>54</v>
       </c>
@@ -3699,7 +3699,7 @@
         <v>1.9444444444444445E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>56</v>
       </c>
@@ -3728,7 +3728,7 @@
         <v>6.5277777777777782E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>58</v>
       </c>
@@ -3757,7 +3757,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>59</v>
       </c>
@@ -3786,7 +3786,7 @@
         <v>2.9861111111111113E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>61</v>
       </c>
@@ -3815,7 +3815,7 @@
         <v>5.4166666666666669E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>63</v>
       </c>
@@ -3844,7 +3844,7 @@
         <v>6.7361111111111108E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>65</v>
       </c>
@@ -3873,7 +3873,7 @@
         <v>3.4027777777777775E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
         <v>66</v>
       </c>
@@ -3902,7 +3902,7 @@
         <v>2.2222222222222223E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
         <v>68</v>
       </c>
@@ -3931,7 +3931,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="10"/>
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
@@ -3944,7 +3944,7 @@
       <c r="H29" s="10"/>
       <c r="I29" s="10"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
         <v>70</v>
       </c>
@@ -3973,7 +3973,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>73</v>
       </c>
@@ -4002,7 +4002,7 @@
         <v>5.6250000000000001E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
         <v>75</v>
       </c>
@@ -4031,7 +4031,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
         <v>77</v>
       </c>
@@ -4060,7 +4060,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
         <v>79</v>
       </c>
@@ -4089,7 +4089,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
         <v>81</v>
       </c>
@@ -4118,7 +4118,7 @@
         <v>2.4305555555555556E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
         <v>82</v>
       </c>
@@ -4147,7 +4147,7 @@
         <v>6.0416666666666667E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
         <v>84</v>
       </c>
@@ -4176,7 +4176,7 @@
         <v>6.1805555555555558E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
         <v>85</v>
       </c>
@@ -4205,7 +4205,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" s="4" t="s">
         <v>86</v>
       </c>
@@ -4234,7 +4234,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="s">
         <v>88</v>
       </c>
@@ -4263,7 +4263,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="s">
         <v>89</v>
       </c>
@@ -4292,7 +4292,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="s">
         <v>91</v>
       </c>
@@ -4321,7 +4321,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">
         <v>93</v>
       </c>
@@ -4350,7 +4350,7 @@
         <v>5.1388888888888887E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
         <v>94</v>
       </c>
@@ -4379,7 +4379,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
         <v>95</v>
       </c>
@@ -4408,7 +4408,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
         <v>96</v>
       </c>
@@ -4437,7 +4437,7 @@
         <v>6.3888888888888884E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="s">
         <v>97</v>
       </c>
@@ -4466,7 +4466,7 @@
         <v>4.8611111111111112E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="s">
         <v>99</v>
       </c>
@@ -4495,7 +4495,7 @@
         <v>5.2083333333333336E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
         <v>100</v>
       </c>
@@ -4524,7 +4524,7 @@
         <v>3.9583333333333331E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
         <v>102</v>
       </c>
@@ -4553,7 +4553,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="s">
         <v>104</v>
       </c>
@@ -4582,7 +4582,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" s="4" t="s">
         <v>105</v>
       </c>
@@ -4611,7 +4611,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="s">
         <v>107</v>
       </c>
@@ -4640,7 +4640,7 @@
         <v>6.1805555555555558E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" s="4" t="s">
         <v>108</v>
       </c>
@@ -4669,7 +4669,7 @@
         <v>5.9722222222222225E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="s">
         <v>110</v>
       </c>
@@ -4698,162 +4698,162 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C57" s="9" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C58" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C59" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C60" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C61" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C62" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C63" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C64" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="65" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C65" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="66" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C66" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="67" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C67" s="4" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="68" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C68" s="4" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="69" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C69" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="70" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C70" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="71" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C71" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="72" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C72" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="73" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C73" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="74" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C74" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="75" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C75" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="76" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C76" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="77" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C77" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="78" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="78" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C78" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="79" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="79" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C79" s="4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="80" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="80" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C80" s="4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="81" spans="3:6" x14ac:dyDescent="0.45">
+    <row r="81" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C81" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="82" spans="3:6" x14ac:dyDescent="0.45">
+    <row r="82" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C82" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="83" spans="3:6" x14ac:dyDescent="0.45">
+    <row r="83" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C83" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="84" spans="3:6" x14ac:dyDescent="0.45">
+    <row r="84" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C84" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="85" spans="3:6" x14ac:dyDescent="0.45">
+    <row r="85" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C85" s="4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="86" spans="3:6" x14ac:dyDescent="0.45">
+    <row r="86" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C86" s="4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="87" spans="3:6" x14ac:dyDescent="0.45">
+    <row r="87" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C87" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="95" spans="3:6" x14ac:dyDescent="0.45">
+    <row r="95" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C95" t="s">
         <v>118</v>
       </c>
@@ -4865,7 +4865,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="3:6" x14ac:dyDescent="0.45">
+    <row r="96" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C96" t="s">
         <v>145</v>
       </c>
@@ -4877,7 +4877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="3:6" x14ac:dyDescent="0.45">
+    <row r="97" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C97" t="s">
         <v>115</v>
       </c>
@@ -4889,7 +4889,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="98" spans="3:6" x14ac:dyDescent="0.45">
+    <row r="98" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C98" t="s">
         <v>116</v>
       </c>
@@ -4901,7 +4901,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="3:6" x14ac:dyDescent="0.45">
+    <row r="99" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C99" t="s">
         <v>117</v>
       </c>
@@ -4913,12 +4913,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="3:6" x14ac:dyDescent="0.45">
+    <row r="100" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C100" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="101" spans="3:6" x14ac:dyDescent="0.45">
+    <row r="101" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C101" t="s">
         <v>118</v>
       </c>
@@ -4930,7 +4930,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="3:6" x14ac:dyDescent="0.45">
+    <row r="102" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C102" t="s">
         <v>116</v>
       </c>
@@ -4942,7 +4942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="3:6" x14ac:dyDescent="0.45">
+    <row r="103" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C103" t="s">
         <v>119</v>
       </c>
@@ -4954,7 +4954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="3:6" x14ac:dyDescent="0.45">
+    <row r="104" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C104" t="s">
         <v>115</v>
       </c>
@@ -4966,7 +4966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="3:6" x14ac:dyDescent="0.45">
+    <row r="105" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C105" t="s">
         <v>118</v>
       </c>
@@ -4978,7 +4978,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="106" spans="3:6" x14ac:dyDescent="0.45">
+    <row r="106" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C106" t="s">
         <v>120</v>
       </c>
@@ -4990,7 +4990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="3:6" x14ac:dyDescent="0.45">
+    <row r="107" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C107" t="s">
         <v>121</v>
       </c>
@@ -5002,7 +5002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="3:6" x14ac:dyDescent="0.45">
+    <row r="108" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C108" t="s">
         <v>115</v>
       </c>
@@ -5014,7 +5014,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="109" spans="3:6" x14ac:dyDescent="0.45">
+    <row r="109" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C109" t="s">
         <v>122</v>
       </c>
@@ -5026,7 +5026,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="110" spans="3:6" x14ac:dyDescent="0.45">
+    <row r="110" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C110" t="s">
         <v>123</v>
       </c>
@@ -5038,7 +5038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="3:6" x14ac:dyDescent="0.45">
+    <row r="111" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C111" t="s">
         <v>116</v>
       </c>
@@ -5050,7 +5050,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="112" spans="3:6" x14ac:dyDescent="0.45">
+    <row r="112" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C112" t="s">
         <v>124</v>
       </c>
@@ -5062,7 +5062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="3:6" x14ac:dyDescent="0.45">
+    <row r="113" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C113" t="s">
         <v>125</v>
       </c>
@@ -5074,7 +5074,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="114" spans="3:6" x14ac:dyDescent="0.45">
+    <row r="114" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C114" t="s">
         <v>115</v>
       </c>
@@ -5086,7 +5086,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="115" spans="3:6" x14ac:dyDescent="0.45">
+    <row r="115" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C115" t="s">
         <v>126</v>
       </c>
@@ -5098,7 +5098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="3:6" x14ac:dyDescent="0.45">
+    <row r="116" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C116" t="s">
         <v>127</v>
       </c>
@@ -5110,7 +5110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="3:6" x14ac:dyDescent="0.45">
+    <row r="117" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C117" t="s">
         <v>118</v>
       </c>
@@ -5122,7 +5122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="3:6" x14ac:dyDescent="0.45">
+    <row r="118" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C118" t="s">
         <v>123</v>
       </c>
@@ -5134,7 +5134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="3:6" x14ac:dyDescent="0.45">
+    <row r="119" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C119" t="s">
         <v>128</v>
       </c>
@@ -5146,7 +5146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="3:6" x14ac:dyDescent="0.45">
+    <row r="120" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C120" t="s">
         <v>126</v>
       </c>
@@ -5158,7 +5158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="3:6" x14ac:dyDescent="0.45">
+    <row r="121" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C121" t="s">
         <v>129</v>
       </c>
@@ -5170,7 +5170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="3:6" x14ac:dyDescent="0.45">
+    <row r="122" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C122" t="s">
         <v>130</v>
       </c>
@@ -5182,7 +5182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="3:6" x14ac:dyDescent="0.45">
+    <row r="123" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C123" t="s">
         <v>131</v>
       </c>
@@ -5194,7 +5194,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="124" spans="3:6" x14ac:dyDescent="0.45">
+    <row r="124" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C124" t="s">
         <v>132</v>
       </c>
@@ -5206,7 +5206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="3:6" x14ac:dyDescent="0.45">
+    <row r="125" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C125" t="s">
         <v>133</v>
       </c>
@@ -5218,7 +5218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="3:6" x14ac:dyDescent="0.45">
+    <row r="126" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C126" t="s">
         <v>126</v>
       </c>
@@ -5230,108 +5230,112 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="3:6" x14ac:dyDescent="0.45">
+    <row r="127" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C127" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="128" spans="3:6" x14ac:dyDescent="0.45">
+    <row r="128" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C128" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="129" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="129" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C129" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="130" spans="3:3" x14ac:dyDescent="0.45">
+      <c r="F129">
+        <f>MAX(F95:F126)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="130" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C130" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="131" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="131" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C131" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="132" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="132" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C132" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="133" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="133" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C133" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="134" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="134" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C134" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="135" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="135" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C135" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="136" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="136" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C136" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="137" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="137" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C137" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="138" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="138" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C138" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="139" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="139" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C139" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="140" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="140" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C140" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="141" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="141" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C141" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="142" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="142" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C142" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="143" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="143" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C143" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="144" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="144" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C144" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="145" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="145" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C145" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="146" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="146" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C146" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="147" spans="3:3" x14ac:dyDescent="0.45">
-      <c r="C147" s="17"/>
+    <row r="147" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C147" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>